<commit_message>
add searching files script
</commit_message>
<xml_diff>
--- a/CS-BRAC055U007 - Copy.xlsx
+++ b/CS-BRAC055U007 - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idexonline-my.sharepoint.com/personal/cmerkle_idexcorp_com/Documents/Desktop/Configsheet_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="13_ncr:1_{112C743C-75E5-4915-9EF8-8D778495E2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99C1E97F-5C43-434C-968C-8D6F74123B2F}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{112C743C-75E5-4915-9EF8-8D778495E2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95137E7A-58E3-4AFD-A72B-3DC4D16D0CC8}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15720" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,7 +545,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3822" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3822" uniqueCount="312">
   <si>
     <t>Rev.</t>
   </si>
@@ -1542,6 +1542,9 @@
   </si>
   <si>
     <t>CH-004390</t>
+  </si>
+  <si>
+    <t>Check Valve Title</t>
   </si>
 </sst>
 </file>
@@ -7323,7 +7326,7 @@
   <dimension ref="A1:AA102"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:R1"/>
+      <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7629,7 +7632,7 @@
     <row r="12" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="414"/>
       <c r="B12" s="498" t="s">
-        <v>20</v>
+        <v>311</v>
       </c>
       <c r="C12" s="499"/>
       <c r="D12" s="499"/>

</xml_diff>